<commit_message>
Remove error folder Admin-site
</commit_message>
<xml_diff>
--- a/Planning-Assignment.xlsx
+++ b/Planning-Assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b7e72e79f608150/Máy tính/Assignment-Ecommerce-Rookie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b7e72e79f608150/Máy tính/Assignment-Ecommerce-Rookie-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{940DEEB6-91B8-426D-9A09-1CE5F3826108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F7CBAAD4-E1D1-4EC4-8A19-E0E811C63149}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{940DEEB6-91B8-426D-9A09-1CE5F3826108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{27B08FDC-368D-4273-AC62-32D15BB9C2BB}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="16200" windowHeight="9970" xr2:uid="{E0C963B1-BBD0-4C02-A4A1-F38FABEABE73}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{E0C963B1-BBD0-4C02-A4A1-F38FABEABE73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Tên chức năng</t>
   </si>
@@ -198,16 +198,13 @@
     <t>Các chức năng hệ thống</t>
   </si>
   <si>
-    <t>Code product-detail</t>
-  </si>
-  <si>
-    <t>check</t>
-  </si>
-  <si>
-    <t>Xử lý file database</t>
-  </si>
-  <si>
     <t>Todolist - (10-10-2022)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sắp xếp sản phẩm </t>
   </si>
 </sst>
 </file>
@@ -285,10 +282,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -604,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560C8A24-99FF-4BCC-9706-01297FBA529C}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,10 +618,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -653,6 +650,9 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
       <c r="E3" t="s">
         <v>33</v>
       </c>
@@ -675,6 +675,9 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
       <c r="F5" t="s">
         <v>28</v>
       </c>
@@ -683,6 +686,9 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
       <c r="F6" t="s">
         <v>29</v>
       </c>
@@ -691,6 +697,9 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
       <c r="E7" t="s">
         <v>36</v>
       </c>
@@ -713,6 +722,9 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
       <c r="F9" t="s">
         <v>32</v>
       </c>
@@ -721,6 +733,9 @@
       <c r="B10" t="s">
         <v>9</v>
       </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
       <c r="E10" t="s">
         <v>38</v>
       </c>
@@ -732,6 +747,9 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
       <c r="F11" t="s">
         <v>42</v>
       </c>
@@ -740,6 +758,9 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
       <c r="F12" t="s">
         <v>39</v>
       </c>
@@ -751,6 +772,9 @@
       <c r="B13" t="s">
         <v>13</v>
       </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
       <c r="F13" t="s">
         <v>40</v>
       </c>
@@ -759,6 +783,9 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
       <c r="E14" t="s">
         <v>43</v>
       </c>
@@ -770,6 +797,9 @@
       <c r="B15" t="s">
         <v>15</v>
       </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
       <c r="F15" t="s">
         <v>45</v>
       </c>
@@ -778,6 +808,9 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
       <c r="E16" t="s">
         <v>46</v>
       </c>
@@ -789,6 +822,9 @@
       <c r="B17" t="s">
         <v>17</v>
       </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
       <c r="E17" t="s">
         <v>49</v>
       </c>
@@ -798,7 +834,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
       </c>
       <c r="F18" t="s">
         <v>50</v>
@@ -806,7 +845,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
       </c>
       <c r="F19" t="s">
         <v>51</v>
@@ -814,58 +856,53 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>23</v>
+      <c r="C22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.5">
-      <c r="A26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>